<commit_message>
version 2: Add Feature -> let manager to create schedule for department member
</commit_message>
<xml_diff>
--- a/DB Schema.xlsx
+++ b/DB Schema.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>MESSAGE_SCHEDULE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -117,10 +117,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>nvarchar(1) null or 1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>last_timestamp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -146,6 +142,26 @@
   </si>
   <si>
     <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message_Manager</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP_UNIT_ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>doc.doc.user_job_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nvarchar(1) null or '1'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -189,8 +205,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -471,15 +493,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="2" max="2" width="19.25" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="17.5" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
@@ -517,10 +540,10 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I1" t="s">
         <v>15</v>
@@ -547,10 +570,10 @@
         <v>23</v>
       </c>
       <c r="Q1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -570,7 +593,7 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -582,7 +605,7 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
@@ -600,11 +623,33 @@
         <v>18</v>
       </c>
       <c r="Q2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="R2" t="s">
-        <v>26</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>